<commit_message>
Actualización de Planificación 10-09-2021
</commit_message>
<xml_diff>
--- a/PlanCarlosSelman SOPESA.xlsx
+++ b/PlanCarlosSelman SOPESA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carli\Documents\CICLO ESCOLAR 2021\Prácticas 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carli\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3188,8 +3188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M108"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A61" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="J77" sqref="J77"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A85" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4316,7 +4316,7 @@
         <v>44453</v>
       </c>
       <c r="H61" s="144">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.25">
@@ -4529,7 +4529,7 @@
         <v>44470</v>
       </c>
       <c r="H74" s="144">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
@@ -5029,8 +5029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AH28"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Actualización de planificación 17-09-2021
</commit_message>
<xml_diff>
--- a/PlanCarlosSelman SOPESA.xlsx
+++ b/PlanCarlosSelman SOPESA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carli\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carli\Documents\CICLO ESCOLAR 2021\Prácticas 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3188,8 +3188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M108"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A85" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A67" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4529,7 +4529,7 @@
         <v>44470</v>
       </c>
       <c r="H74" s="144">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Actualización de Planificación 24-09-2021
</commit_message>
<xml_diff>
--- a/PlanCarlosSelman SOPESA.xlsx
+++ b/PlanCarlosSelman SOPESA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carli\Documents\CICLO ESCOLAR 2021\Prácticas 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sopesaMeet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1769,23 +1769,257 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="15" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="14" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1796,238 +2030,64 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="14" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="15" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2041,66 +2101,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3188,8 +3188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M108"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A67" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A58" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3210,103 +3210,103 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="177"/>
-      <c r="C2" s="178"/>
-      <c r="D2" s="183" t="s">
+      <c r="B2" s="122"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="184"/>
-      <c r="F2" s="184"/>
-      <c r="G2" s="184"/>
-      <c r="H2" s="162"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="163"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="177" t="s">
+      <c r="J2" s="122" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="199"/>
-      <c r="L2" s="178"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="124"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="179"/>
-      <c r="C3" s="180"/>
-      <c r="D3" s="158" t="s">
+      <c r="B3" s="125"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="159" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="159"/>
-      <c r="F3" s="159"/>
-      <c r="G3" s="159"/>
-      <c r="H3" s="163"/>
-      <c r="J3" s="179" t="s">
+      <c r="E3" s="160"/>
+      <c r="F3" s="160"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="164"/>
+      <c r="J3" s="125" t="s">
         <v>68</v>
       </c>
-      <c r="K3" s="200"/>
-      <c r="L3" s="180"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="127"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="179"/>
-      <c r="C4" s="180"/>
-      <c r="D4" s="185" t="s">
+      <c r="B4" s="125"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="178" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="186"/>
-      <c r="F4" s="186"/>
-      <c r="G4" s="186"/>
-      <c r="H4" s="163"/>
-      <c r="J4" s="179" t="s">
+      <c r="E4" s="179"/>
+      <c r="F4" s="179"/>
+      <c r="G4" s="179"/>
+      <c r="H4" s="164"/>
+      <c r="J4" s="125" t="s">
         <v>69</v>
       </c>
-      <c r="K4" s="200"/>
-      <c r="L4" s="180"/>
+      <c r="K4" s="126"/>
+      <c r="L4" s="127"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="179"/>
-      <c r="C5" s="180"/>
-      <c r="D5" s="158" t="s">
+      <c r="B5" s="125"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="159" t="s">
         <v>179</v>
       </c>
-      <c r="E5" s="159"/>
-      <c r="F5" s="159"/>
-      <c r="G5" s="159"/>
-      <c r="H5" s="163"/>
-      <c r="J5" s="181" t="s">
+      <c r="E5" s="160"/>
+      <c r="F5" s="160"/>
+      <c r="G5" s="160"/>
+      <c r="H5" s="164"/>
+      <c r="J5" s="138" t="s">
         <v>70</v>
       </c>
-      <c r="K5" s="201"/>
-      <c r="L5" s="182"/>
+      <c r="K5" s="139"/>
+      <c r="L5" s="140"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="179"/>
-      <c r="C6" s="180"/>
-      <c r="D6" s="187" t="s">
+      <c r="B6" s="125"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="180" t="s">
         <v>181</v>
       </c>
-      <c r="E6" s="188"/>
-      <c r="F6" s="188"/>
-      <c r="G6" s="189"/>
-      <c r="H6" s="163"/>
+      <c r="E6" s="181"/>
+      <c r="F6" s="181"/>
+      <c r="G6" s="182"/>
+      <c r="H6" s="164"/>
     </row>
     <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="181"/>
-      <c r="C7" s="182"/>
-      <c r="D7" s="160" t="s">
+      <c r="B7" s="138"/>
+      <c r="C7" s="140"/>
+      <c r="D7" s="161" t="s">
         <v>180</v>
       </c>
-      <c r="E7" s="161"/>
-      <c r="F7" s="161"/>
-      <c r="G7" s="161"/>
-      <c r="H7" s="164"/>
-      <c r="J7" s="202" t="s">
+      <c r="E7" s="162"/>
+      <c r="F7" s="162"/>
+      <c r="G7" s="162"/>
+      <c r="H7" s="165"/>
+      <c r="J7" s="141" t="s">
         <v>75</v>
       </c>
-      <c r="K7" s="203"/>
-      <c r="L7" s="204"/>
+      <c r="K7" s="142"/>
+      <c r="L7" s="143"/>
     </row>
     <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="175" t="s">
+      <c r="B8" s="170" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="176"/>
+      <c r="C8" s="171"/>
       <c r="D8" s="11" t="s">
         <v>33</v>
       </c>
@@ -3322,36 +3322,36 @@
       <c r="H8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="205"/>
-      <c r="K8" s="206"/>
-      <c r="L8" s="207"/>
+      <c r="J8" s="144"/>
+      <c r="K8" s="145"/>
+      <c r="L8" s="146"/>
     </row>
     <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="123">
+      <c r="B9" s="172">
         <v>1</v>
       </c>
-      <c r="C9" s="124"/>
+      <c r="C9" s="173"/>
       <c r="D9" s="35" t="s">
         <v>139</v>
       </c>
       <c r="E9" s="93" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="125">
+      <c r="F9" s="130">
         <v>44424</v>
       </c>
-      <c r="G9" s="135">
+      <c r="G9" s="156">
         <v>44424</v>
       </c>
-      <c r="H9" s="144">
+      <c r="H9" s="134">
         <v>1</v>
       </c>
-      <c r="J9" s="177"/>
-      <c r="K9" s="199"/>
-      <c r="L9" s="178"/>
+      <c r="J9" s="122"/>
+      <c r="K9" s="123"/>
+      <c r="L9" s="124"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="139"/>
+      <c r="B10" s="183"/>
       <c r="C10" s="70" t="s">
         <v>40</v>
       </c>
@@ -3361,15 +3361,15 @@
       <c r="E10" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="126"/>
-      <c r="G10" s="197"/>
-      <c r="H10" s="145"/>
-      <c r="J10" s="179"/>
-      <c r="K10" s="200"/>
-      <c r="L10" s="180"/>
+      <c r="F10" s="131"/>
+      <c r="G10" s="157"/>
+      <c r="H10" s="136"/>
+      <c r="J10" s="125"/>
+      <c r="K10" s="126"/>
+      <c r="L10" s="127"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="139"/>
+      <c r="B11" s="183"/>
       <c r="C11" s="68" t="s">
         <v>39</v>
       </c>
@@ -3379,15 +3379,15 @@
       <c r="E11" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="126"/>
-      <c r="G11" s="197"/>
-      <c r="H11" s="145"/>
-      <c r="J11" s="179"/>
-      <c r="K11" s="200"/>
-      <c r="L11" s="180"/>
+      <c r="F11" s="131"/>
+      <c r="G11" s="157"/>
+      <c r="H11" s="136"/>
+      <c r="J11" s="125"/>
+      <c r="K11" s="126"/>
+      <c r="L11" s="127"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="139"/>
+      <c r="B12" s="183"/>
       <c r="C12" s="69" t="s">
         <v>41</v>
       </c>
@@ -3397,15 +3397,15 @@
       <c r="E12" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="126"/>
-      <c r="G12" s="197"/>
-      <c r="H12" s="145"/>
-      <c r="J12" s="179"/>
-      <c r="K12" s="200"/>
-      <c r="L12" s="180"/>
+      <c r="F12" s="131"/>
+      <c r="G12" s="157"/>
+      <c r="H12" s="136"/>
+      <c r="J12" s="125"/>
+      <c r="K12" s="126"/>
+      <c r="L12" s="127"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="139"/>
+      <c r="B13" s="183"/>
       <c r="C13" s="68" t="s">
         <v>42</v>
       </c>
@@ -3415,15 +3415,15 @@
       <c r="E13" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="126"/>
-      <c r="G13" s="197"/>
-      <c r="H13" s="145"/>
-      <c r="J13" s="179"/>
-      <c r="K13" s="200"/>
-      <c r="L13" s="180"/>
+      <c r="F13" s="131"/>
+      <c r="G13" s="157"/>
+      <c r="H13" s="136"/>
+      <c r="J13" s="125"/>
+      <c r="K13" s="126"/>
+      <c r="L13" s="127"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="139"/>
+      <c r="B14" s="183"/>
       <c r="C14" s="67" t="s">
         <v>43</v>
       </c>
@@ -3433,15 +3433,15 @@
       <c r="E14" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="126"/>
-      <c r="G14" s="197"/>
-      <c r="H14" s="145"/>
-      <c r="J14" s="179"/>
-      <c r="K14" s="200"/>
-      <c r="L14" s="180"/>
+      <c r="F14" s="131"/>
+      <c r="G14" s="157"/>
+      <c r="H14" s="136"/>
+      <c r="J14" s="125"/>
+      <c r="K14" s="126"/>
+      <c r="L14" s="127"/>
     </row>
     <row r="15" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="139"/>
+      <c r="B15" s="183"/>
       <c r="C15" s="82" t="s">
         <v>132</v>
       </c>
@@ -3451,271 +3451,271 @@
       <c r="E15" s="88" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="127"/>
-      <c r="G15" s="198"/>
-      <c r="H15" s="146"/>
-      <c r="J15" s="179"/>
-      <c r="K15" s="200"/>
-      <c r="L15" s="180"/>
+      <c r="F15" s="132"/>
+      <c r="G15" s="158"/>
+      <c r="H15" s="137"/>
+      <c r="J15" s="125"/>
+      <c r="K15" s="126"/>
+      <c r="L15" s="127"/>
     </row>
     <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="123">
+      <c r="B16" s="172">
         <v>2</v>
       </c>
-      <c r="C16" s="124"/>
+      <c r="C16" s="173"/>
       <c r="D16" s="90" t="s">
         <v>91</v>
       </c>
       <c r="E16" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="125">
+      <c r="F16" s="130">
         <v>44424</v>
       </c>
-      <c r="G16" s="135">
+      <c r="G16" s="156">
         <v>44424</v>
       </c>
-      <c r="H16" s="144">
+      <c r="H16" s="134">
         <v>1</v>
       </c>
-      <c r="J16" s="179"/>
-      <c r="K16" s="200"/>
-      <c r="L16" s="180"/>
+      <c r="J16" s="125"/>
+      <c r="K16" s="126"/>
+      <c r="L16" s="127"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="139"/>
+      <c r="B17" s="183"/>
       <c r="C17" s="63" t="s">
         <v>48</v>
       </c>
       <c r="D17" s="89" t="s">
         <v>168</v>
       </c>
-      <c r="E17" s="131" t="s">
+      <c r="E17" s="168" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="133"/>
-      <c r="G17" s="136"/>
-      <c r="H17" s="145"/>
-      <c r="J17" s="181" t="s">
+      <c r="F17" s="147"/>
+      <c r="G17" s="201"/>
+      <c r="H17" s="136"/>
+      <c r="J17" s="138" t="s">
         <v>72</v>
       </c>
-      <c r="K17" s="201"/>
-      <c r="L17" s="182"/>
+      <c r="K17" s="139"/>
+      <c r="L17" s="140"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="139"/>
+      <c r="B18" s="183"/>
       <c r="C18" s="64" t="s">
         <v>49</v>
       </c>
       <c r="D18" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="E18" s="131"/>
-      <c r="F18" s="133"/>
-      <c r="G18" s="136"/>
-      <c r="H18" s="145"/>
-      <c r="J18" s="177"/>
-      <c r="K18" s="199"/>
-      <c r="L18" s="178"/>
+      <c r="E18" s="168"/>
+      <c r="F18" s="147"/>
+      <c r="G18" s="201"/>
+      <c r="H18" s="136"/>
+      <c r="J18" s="122"/>
+      <c r="K18" s="123"/>
+      <c r="L18" s="124"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="139"/>
+      <c r="B19" s="183"/>
       <c r="C19" s="63" t="s">
         <v>50</v>
       </c>
       <c r="D19" s="60" t="s">
         <v>170</v>
       </c>
-      <c r="E19" s="132"/>
-      <c r="F19" s="133"/>
-      <c r="G19" s="136"/>
-      <c r="H19" s="145"/>
-      <c r="J19" s="179"/>
-      <c r="K19" s="200"/>
-      <c r="L19" s="180"/>
+      <c r="E19" s="191"/>
+      <c r="F19" s="147"/>
+      <c r="G19" s="201"/>
+      <c r="H19" s="136"/>
+      <c r="J19" s="125"/>
+      <c r="K19" s="126"/>
+      <c r="L19" s="127"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="139"/>
+      <c r="B20" s="183"/>
       <c r="C20" s="64" t="s">
         <v>51</v>
       </c>
       <c r="D20" s="62" t="s">
         <v>171</v>
       </c>
-      <c r="E20" s="130" t="s">
+      <c r="E20" s="208" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="133"/>
-      <c r="G20" s="136"/>
-      <c r="H20" s="145"/>
-      <c r="J20" s="179"/>
-      <c r="K20" s="200"/>
-      <c r="L20" s="180"/>
+      <c r="F20" s="147"/>
+      <c r="G20" s="201"/>
+      <c r="H20" s="136"/>
+      <c r="J20" s="125"/>
+      <c r="K20" s="126"/>
+      <c r="L20" s="127"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="139"/>
+      <c r="B21" s="183"/>
       <c r="C21" s="65" t="s">
         <v>52</v>
       </c>
       <c r="D21" s="60" t="s">
         <v>172</v>
       </c>
-      <c r="E21" s="131"/>
-      <c r="F21" s="133"/>
-      <c r="G21" s="136"/>
-      <c r="H21" s="145"/>
-      <c r="J21" s="179"/>
-      <c r="K21" s="200"/>
-      <c r="L21" s="180"/>
+      <c r="E21" s="168"/>
+      <c r="F21" s="147"/>
+      <c r="G21" s="201"/>
+      <c r="H21" s="136"/>
+      <c r="J21" s="125"/>
+      <c r="K21" s="126"/>
+      <c r="L21" s="127"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="139"/>
+      <c r="B22" s="183"/>
       <c r="C22" s="66" t="s">
         <v>53</v>
       </c>
       <c r="D22" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="E22" s="132"/>
-      <c r="F22" s="133"/>
-      <c r="G22" s="136"/>
-      <c r="H22" s="145"/>
-      <c r="J22" s="179"/>
-      <c r="K22" s="200"/>
-      <c r="L22" s="180"/>
+      <c r="E22" s="191"/>
+      <c r="F22" s="147"/>
+      <c r="G22" s="201"/>
+      <c r="H22" s="136"/>
+      <c r="J22" s="125"/>
+      <c r="K22" s="126"/>
+      <c r="L22" s="127"/>
     </row>
     <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="139"/>
+      <c r="B23" s="183"/>
       <c r="C23" s="81" t="s">
         <v>54</v>
       </c>
       <c r="D23" s="60" t="s">
         <v>174</v>
       </c>
-      <c r="E23" s="130" t="s">
+      <c r="E23" s="208" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="133"/>
-      <c r="G23" s="136"/>
-      <c r="H23" s="145"/>
-      <c r="J23" s="181" t="s">
+      <c r="F23" s="147"/>
+      <c r="G23" s="201"/>
+      <c r="H23" s="136"/>
+      <c r="J23" s="138" t="s">
         <v>73</v>
       </c>
-      <c r="K23" s="201"/>
-      <c r="L23" s="182"/>
+      <c r="K23" s="139"/>
+      <c r="L23" s="140"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="190"/>
-      <c r="C24" s="191"/>
+      <c r="B24" s="184"/>
+      <c r="C24" s="185"/>
       <c r="D24" s="73" t="s">
         <v>90</v>
       </c>
-      <c r="E24" s="131"/>
-      <c r="F24" s="133"/>
-      <c r="G24" s="136"/>
-      <c r="H24" s="145"/>
-      <c r="J24" s="177"/>
-      <c r="K24" s="199"/>
-      <c r="L24" s="178"/>
+      <c r="E24" s="168"/>
+      <c r="F24" s="147"/>
+      <c r="G24" s="201"/>
+      <c r="H24" s="136"/>
+      <c r="J24" s="122"/>
+      <c r="K24" s="123"/>
+      <c r="L24" s="124"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="190"/>
-      <c r="C25" s="191"/>
+      <c r="B25" s="184"/>
+      <c r="C25" s="185"/>
       <c r="D25" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="131"/>
-      <c r="F25" s="133"/>
-      <c r="G25" s="136"/>
-      <c r="H25" s="145"/>
-      <c r="J25" s="179"/>
-      <c r="K25" s="200"/>
-      <c r="L25" s="180"/>
+      <c r="E25" s="168"/>
+      <c r="F25" s="147"/>
+      <c r="G25" s="201"/>
+      <c r="H25" s="136"/>
+      <c r="J25" s="125"/>
+      <c r="K25" s="126"/>
+      <c r="L25" s="127"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="190"/>
-      <c r="C26" s="191"/>
+      <c r="B26" s="184"/>
+      <c r="C26" s="185"/>
       <c r="D26" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="E26" s="131"/>
-      <c r="F26" s="133"/>
-      <c r="G26" s="136"/>
-      <c r="H26" s="145"/>
-      <c r="J26" s="179"/>
-      <c r="K26" s="200"/>
-      <c r="L26" s="180"/>
+      <c r="E26" s="168"/>
+      <c r="F26" s="147"/>
+      <c r="G26" s="201"/>
+      <c r="H26" s="136"/>
+      <c r="J26" s="125"/>
+      <c r="K26" s="126"/>
+      <c r="L26" s="127"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="190"/>
-      <c r="C27" s="191"/>
+      <c r="B27" s="184"/>
+      <c r="C27" s="185"/>
       <c r="D27" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="E27" s="131"/>
-      <c r="F27" s="133"/>
-      <c r="G27" s="136"/>
-      <c r="H27" s="145"/>
-      <c r="J27" s="179"/>
-      <c r="K27" s="200"/>
-      <c r="L27" s="180"/>
+      <c r="E27" s="168"/>
+      <c r="F27" s="147"/>
+      <c r="G27" s="201"/>
+      <c r="H27" s="136"/>
+      <c r="J27" s="125"/>
+      <c r="K27" s="126"/>
+      <c r="L27" s="127"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="190"/>
-      <c r="C28" s="191"/>
+      <c r="B28" s="184"/>
+      <c r="C28" s="185"/>
       <c r="D28" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="131"/>
-      <c r="F28" s="133"/>
-      <c r="G28" s="136"/>
-      <c r="H28" s="145"/>
-      <c r="J28" s="179"/>
-      <c r="K28" s="200"/>
-      <c r="L28" s="180"/>
+      <c r="E28" s="168"/>
+      <c r="F28" s="147"/>
+      <c r="G28" s="201"/>
+      <c r="H28" s="136"/>
+      <c r="J28" s="125"/>
+      <c r="K28" s="126"/>
+      <c r="L28" s="127"/>
     </row>
     <row r="29" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="192"/>
-      <c r="C29" s="193"/>
+      <c r="B29" s="186"/>
+      <c r="C29" s="187"/>
       <c r="D29" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="E29" s="131"/>
-      <c r="F29" s="134"/>
-      <c r="G29" s="137"/>
-      <c r="H29" s="146"/>
-      <c r="J29" s="181" t="s">
+      <c r="E29" s="168"/>
+      <c r="F29" s="148"/>
+      <c r="G29" s="202"/>
+      <c r="H29" s="137"/>
+      <c r="J29" s="138" t="s">
         <v>74</v>
       </c>
-      <c r="K29" s="201"/>
-      <c r="L29" s="182"/>
+      <c r="K29" s="139"/>
+      <c r="L29" s="140"/>
     </row>
     <row r="30" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="147">
+      <c r="B30" s="174">
         <v>3</v>
       </c>
-      <c r="C30" s="149"/>
+      <c r="C30" s="175"/>
       <c r="D30" s="96" t="s">
         <v>84</v>
       </c>
       <c r="E30" s="93" t="s">
         <v>47</v>
       </c>
-      <c r="F30" s="165">
+      <c r="F30" s="155">
         <v>44425</v>
       </c>
-      <c r="G30" s="168">
+      <c r="G30" s="149">
         <v>44425</v>
       </c>
-      <c r="H30" s="171">
+      <c r="H30" s="152">
         <v>1</v>
       </c>
-      <c r="J30" s="177"/>
-      <c r="K30" s="199"/>
-      <c r="L30" s="178"/>
+      <c r="J30" s="122"/>
+      <c r="K30" s="123"/>
+      <c r="L30" s="124"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="194"/>
+      <c r="B31" s="188"/>
       <c r="C31" s="76" t="s">
         <v>55</v>
       </c>
@@ -3726,14 +3726,14 @@
         <v>44</v>
       </c>
       <c r="F31" s="166"/>
-      <c r="G31" s="169"/>
-      <c r="H31" s="172"/>
-      <c r="J31" s="179"/>
-      <c r="K31" s="200"/>
-      <c r="L31" s="180"/>
+      <c r="G31" s="150"/>
+      <c r="H31" s="153"/>
+      <c r="J31" s="125"/>
+      <c r="K31" s="126"/>
+      <c r="L31" s="127"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="195"/>
+      <c r="B32" s="189"/>
       <c r="C32" s="78" t="s">
         <v>56</v>
       </c>
@@ -3744,74 +3744,74 @@
         <v>45</v>
       </c>
       <c r="F32" s="166"/>
-      <c r="G32" s="169"/>
-      <c r="H32" s="172"/>
-      <c r="J32" s="179"/>
-      <c r="K32" s="200"/>
-      <c r="L32" s="180"/>
+      <c r="G32" s="150"/>
+      <c r="H32" s="153"/>
+      <c r="J32" s="125"/>
+      <c r="K32" s="126"/>
+      <c r="L32" s="127"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="195"/>
+      <c r="B33" s="189"/>
       <c r="C33" s="77" t="s">
         <v>57</v>
       </c>
       <c r="D33" s="75" t="s">
         <v>165</v>
       </c>
-      <c r="E33" s="131" t="s">
+      <c r="E33" s="168" t="s">
         <v>44</v>
       </c>
       <c r="F33" s="166"/>
-      <c r="G33" s="169"/>
-      <c r="H33" s="172"/>
-      <c r="J33" s="179"/>
-      <c r="K33" s="200"/>
-      <c r="L33" s="180"/>
+      <c r="G33" s="150"/>
+      <c r="H33" s="153"/>
+      <c r="J33" s="125"/>
+      <c r="K33" s="126"/>
+      <c r="L33" s="127"/>
     </row>
     <row r="34" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="196"/>
+      <c r="B34" s="190"/>
       <c r="C34" s="80" t="s">
         <v>58</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="E34" s="174"/>
+      <c r="E34" s="169"/>
       <c r="F34" s="167"/>
-      <c r="G34" s="170"/>
-      <c r="H34" s="173"/>
-      <c r="J34" s="179"/>
-      <c r="K34" s="200"/>
-      <c r="L34" s="180"/>
+      <c r="G34" s="151"/>
+      <c r="H34" s="154"/>
+      <c r="J34" s="125"/>
+      <c r="K34" s="126"/>
+      <c r="L34" s="127"/>
     </row>
     <row r="35" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="147">
+      <c r="B35" s="174">
         <v>4</v>
       </c>
-      <c r="C35" s="148"/>
+      <c r="C35" s="192"/>
       <c r="D35" s="96" t="s">
         <v>83</v>
       </c>
       <c r="E35" s="93" t="s">
         <v>47</v>
       </c>
-      <c r="F35" s="165">
+      <c r="F35" s="155">
         <v>44425</v>
       </c>
-      <c r="G35" s="168">
+      <c r="G35" s="149">
         <v>44425</v>
       </c>
-      <c r="H35" s="171">
+      <c r="H35" s="152">
         <v>1</v>
       </c>
-      <c r="J35" s="181" t="s">
+      <c r="J35" s="138" t="s">
         <v>79</v>
       </c>
-      <c r="K35" s="201"/>
-      <c r="L35" s="182"/>
+      <c r="K35" s="139"/>
+      <c r="L35" s="140"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="194"/>
+      <c r="B36" s="188"/>
       <c r="C36" s="76" t="s">
         <v>59</v>
       </c>
@@ -3822,14 +3822,14 @@
         <v>44</v>
       </c>
       <c r="F36" s="166"/>
-      <c r="G36" s="169"/>
-      <c r="H36" s="172"/>
-      <c r="J36" s="177"/>
-      <c r="K36" s="199"/>
-      <c r="L36" s="178"/>
+      <c r="G36" s="150"/>
+      <c r="H36" s="153"/>
+      <c r="J36" s="122"/>
+      <c r="K36" s="123"/>
+      <c r="L36" s="124"/>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="195"/>
+      <c r="B37" s="189"/>
       <c r="C37" s="78" t="s">
         <v>60</v>
       </c>
@@ -3840,72 +3840,72 @@
         <v>45</v>
       </c>
       <c r="F37" s="166"/>
-      <c r="G37" s="169"/>
-      <c r="H37" s="172"/>
-      <c r="J37" s="179"/>
-      <c r="K37" s="200"/>
-      <c r="L37" s="180"/>
+      <c r="G37" s="150"/>
+      <c r="H37" s="153"/>
+      <c r="J37" s="125"/>
+      <c r="K37" s="126"/>
+      <c r="L37" s="127"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="195"/>
+      <c r="B38" s="189"/>
       <c r="C38" s="79" t="s">
         <v>61</v>
       </c>
       <c r="D38" s="84" t="s">
         <v>161</v>
       </c>
-      <c r="E38" s="131" t="s">
+      <c r="E38" s="168" t="s">
         <v>44</v>
       </c>
       <c r="F38" s="166"/>
-      <c r="G38" s="169"/>
-      <c r="H38" s="172"/>
-      <c r="J38" s="179"/>
-      <c r="K38" s="200"/>
-      <c r="L38" s="180"/>
+      <c r="G38" s="150"/>
+      <c r="H38" s="153"/>
+      <c r="J38" s="125"/>
+      <c r="K38" s="126"/>
+      <c r="L38" s="127"/>
     </row>
     <row r="39" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="196"/>
+      <c r="B39" s="190"/>
       <c r="C39" s="33" t="s">
         <v>62</v>
       </c>
       <c r="D39" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="E39" s="131"/>
+      <c r="E39" s="168"/>
       <c r="F39" s="167"/>
-      <c r="G39" s="170"/>
-      <c r="H39" s="173"/>
-      <c r="J39" s="179"/>
-      <c r="K39" s="200"/>
-      <c r="L39" s="180"/>
+      <c r="G39" s="151"/>
+      <c r="H39" s="154"/>
+      <c r="J39" s="125"/>
+      <c r="K39" s="126"/>
+      <c r="L39" s="127"/>
     </row>
     <row r="40" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="147">
+      <c r="B40" s="174">
         <v>5</v>
       </c>
-      <c r="C40" s="149"/>
+      <c r="C40" s="175"/>
       <c r="D40" s="96" t="s">
         <v>82</v>
       </c>
       <c r="E40" s="93" t="s">
         <v>119</v>
       </c>
-      <c r="F40" s="125">
+      <c r="F40" s="130">
         <v>44426</v>
       </c>
-      <c r="G40" s="168">
+      <c r="G40" s="149">
         <v>44428</v>
       </c>
-      <c r="H40" s="171">
+      <c r="H40" s="152">
         <v>1</v>
       </c>
-      <c r="J40" s="179"/>
-      <c r="K40" s="200"/>
-      <c r="L40" s="180"/>
+      <c r="J40" s="125"/>
+      <c r="K40" s="126"/>
+      <c r="L40" s="127"/>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B41" s="150"/>
+      <c r="B41" s="193"/>
       <c r="C41" s="76" t="s">
         <v>64</v>
       </c>
@@ -3915,15 +3915,15 @@
       <c r="E41" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="F41" s="133"/>
-      <c r="G41" s="169"/>
-      <c r="H41" s="172"/>
-      <c r="J41" s="179"/>
-      <c r="K41" s="200"/>
-      <c r="L41" s="180"/>
+      <c r="F41" s="147"/>
+      <c r="G41" s="150"/>
+      <c r="H41" s="153"/>
+      <c r="J41" s="125"/>
+      <c r="K41" s="126"/>
+      <c r="L41" s="127"/>
     </row>
     <row r="42" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="150"/>
+      <c r="B42" s="193"/>
       <c r="C42" s="78" t="s">
         <v>65</v>
       </c>
@@ -3933,17 +3933,17 @@
       <c r="E42" s="98" t="s">
         <v>127</v>
       </c>
-      <c r="F42" s="133"/>
-      <c r="G42" s="169"/>
-      <c r="H42" s="172"/>
-      <c r="J42" s="181" t="s">
+      <c r="F42" s="147"/>
+      <c r="G42" s="150"/>
+      <c r="H42" s="153"/>
+      <c r="J42" s="138" t="s">
         <v>204</v>
       </c>
-      <c r="K42" s="201"/>
-      <c r="L42" s="182"/>
+      <c r="K42" s="139"/>
+      <c r="L42" s="140"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B43" s="150"/>
+      <c r="B43" s="193"/>
       <c r="C43" s="79" t="s">
         <v>66</v>
       </c>
@@ -3953,15 +3953,15 @@
       <c r="E43" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="F43" s="133"/>
-      <c r="G43" s="169"/>
-      <c r="H43" s="172"/>
-      <c r="J43" s="177"/>
-      <c r="K43" s="199"/>
-      <c r="L43" s="178"/>
+      <c r="F43" s="147"/>
+      <c r="G43" s="150"/>
+      <c r="H43" s="153"/>
+      <c r="J43" s="122"/>
+      <c r="K43" s="123"/>
+      <c r="L43" s="124"/>
     </row>
     <row r="44" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="151"/>
+      <c r="B44" s="194"/>
       <c r="C44" s="33" t="s">
         <v>67</v>
       </c>
@@ -3971,36 +3971,36 @@
       <c r="E44" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="F44" s="134"/>
-      <c r="G44" s="170"/>
-      <c r="H44" s="173"/>
-      <c r="J44" s="179"/>
-      <c r="K44" s="200"/>
-      <c r="L44" s="180"/>
+      <c r="F44" s="148"/>
+      <c r="G44" s="151"/>
+      <c r="H44" s="154"/>
+      <c r="J44" s="125"/>
+      <c r="K44" s="126"/>
+      <c r="L44" s="127"/>
     </row>
     <row r="45" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="123">
+      <c r="B45" s="172">
         <v>6</v>
       </c>
-      <c r="C45" s="138"/>
+      <c r="C45" s="203"/>
       <c r="D45" s="104" t="s">
         <v>198</v>
       </c>
       <c r="E45" s="93" t="s">
         <v>121</v>
       </c>
-      <c r="F45" s="165">
+      <c r="F45" s="155">
         <v>44431</v>
       </c>
-      <c r="G45" s="135">
+      <c r="G45" s="156">
         <v>44435</v>
       </c>
-      <c r="H45" s="144">
+      <c r="H45" s="134">
         <v>1</v>
       </c>
-      <c r="J45" s="179"/>
-      <c r="K45" s="200"/>
-      <c r="L45" s="180"/>
+      <c r="J45" s="125"/>
+      <c r="K45" s="126"/>
+      <c r="L45" s="127"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" s="14"/>
@@ -4013,12 +4013,12 @@
       <c r="E46" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="F46" s="126"/>
-      <c r="G46" s="197"/>
-      <c r="H46" s="145"/>
-      <c r="J46" s="179"/>
-      <c r="K46" s="200"/>
-      <c r="L46" s="180"/>
+      <c r="F46" s="131"/>
+      <c r="G46" s="157"/>
+      <c r="H46" s="136"/>
+      <c r="J46" s="125"/>
+      <c r="K46" s="126"/>
+      <c r="L46" s="127"/>
     </row>
     <row r="47" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="18"/>
@@ -4031,38 +4031,38 @@
       <c r="E47" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="F47" s="127"/>
-      <c r="G47" s="198"/>
-      <c r="H47" s="146"/>
-      <c r="J47" s="181" t="s">
+      <c r="F47" s="132"/>
+      <c r="G47" s="158"/>
+      <c r="H47" s="137"/>
+      <c r="J47" s="138" t="s">
         <v>76</v>
       </c>
-      <c r="K47" s="201"/>
-      <c r="L47" s="182"/>
+      <c r="K47" s="139"/>
+      <c r="L47" s="140"/>
     </row>
     <row r="48" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="123">
+      <c r="B48" s="172">
         <v>7</v>
       </c>
-      <c r="C48" s="124"/>
+      <c r="C48" s="173"/>
       <c r="D48" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="E48" s="141" t="s">
+      <c r="E48" s="198" t="s">
         <v>44</v>
       </c>
-      <c r="F48" s="125">
+      <c r="F48" s="130">
         <v>44438</v>
       </c>
-      <c r="G48" s="135">
+      <c r="G48" s="156">
         <v>44438</v>
       </c>
-      <c r="H48" s="144">
+      <c r="H48" s="134">
         <v>1</v>
       </c>
-      <c r="J48" s="177"/>
-      <c r="K48" s="199"/>
-      <c r="L48" s="178"/>
+      <c r="J48" s="122"/>
+      <c r="K48" s="123"/>
+      <c r="L48" s="124"/>
     </row>
     <row r="49" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="18"/>
@@ -4072,40 +4072,40 @@
       <c r="D49" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="E49" s="142"/>
-      <c r="F49" s="127"/>
-      <c r="G49" s="198"/>
-      <c r="H49" s="146"/>
-      <c r="J49" s="179"/>
-      <c r="K49" s="200"/>
-      <c r="L49" s="180"/>
+      <c r="E49" s="199"/>
+      <c r="F49" s="132"/>
+      <c r="G49" s="158"/>
+      <c r="H49" s="137"/>
+      <c r="J49" s="125"/>
+      <c r="K49" s="126"/>
+      <c r="L49" s="127"/>
     </row>
     <row r="50" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="123">
+      <c r="B50" s="172">
         <v>8</v>
       </c>
-      <c r="C50" s="124"/>
+      <c r="C50" s="173"/>
       <c r="D50" s="104" t="s">
         <v>92</v>
       </c>
       <c r="E50" s="93" t="s">
         <v>47</v>
       </c>
-      <c r="F50" s="125">
+      <c r="F50" s="130">
         <v>44438</v>
       </c>
-      <c r="G50" s="155">
+      <c r="G50" s="128">
         <v>44438</v>
       </c>
-      <c r="H50" s="144">
+      <c r="H50" s="134">
         <v>1</v>
       </c>
-      <c r="J50" s="179"/>
-      <c r="K50" s="200"/>
-      <c r="L50" s="180"/>
+      <c r="J50" s="125"/>
+      <c r="K50" s="126"/>
+      <c r="L50" s="127"/>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B51" s="152"/>
+      <c r="B51" s="195"/>
       <c r="C51" s="106" t="s">
         <v>142</v>
       </c>
@@ -4115,15 +4115,15 @@
       <c r="E51" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="F51" s="126"/>
-      <c r="G51" s="156"/>
-      <c r="H51" s="145"/>
-      <c r="J51" s="179"/>
-      <c r="K51" s="200"/>
-      <c r="L51" s="180"/>
+      <c r="F51" s="131"/>
+      <c r="G51" s="133"/>
+      <c r="H51" s="136"/>
+      <c r="J51" s="125"/>
+      <c r="K51" s="126"/>
+      <c r="L51" s="127"/>
     </row>
     <row r="52" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="153"/>
+      <c r="B52" s="196"/>
       <c r="C52" s="107" t="s">
         <v>99</v>
       </c>
@@ -4133,17 +4133,17 @@
       <c r="E52" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="F52" s="126"/>
-      <c r="G52" s="156"/>
-      <c r="H52" s="145"/>
-      <c r="J52" s="181" t="s">
+      <c r="F52" s="131"/>
+      <c r="G52" s="133"/>
+      <c r="H52" s="136"/>
+      <c r="J52" s="138" t="s">
         <v>78</v>
       </c>
-      <c r="K52" s="201"/>
-      <c r="L52" s="182"/>
+      <c r="K52" s="139"/>
+      <c r="L52" s="140"/>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B53" s="153"/>
+      <c r="B53" s="196"/>
       <c r="C53" s="108" t="s">
         <v>100</v>
       </c>
@@ -4153,15 +4153,15 @@
       <c r="E53" s="109" t="s">
         <v>46</v>
       </c>
-      <c r="F53" s="126"/>
-      <c r="G53" s="156"/>
-      <c r="H53" s="145"/>
-      <c r="J53" s="177"/>
-      <c r="K53" s="199"/>
-      <c r="L53" s="178"/>
+      <c r="F53" s="131"/>
+      <c r="G53" s="133"/>
+      <c r="H53" s="136"/>
+      <c r="J53" s="122"/>
+      <c r="K53" s="123"/>
+      <c r="L53" s="124"/>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B54" s="153"/>
+      <c r="B54" s="196"/>
       <c r="C54" s="107" t="s">
         <v>101</v>
       </c>
@@ -4171,15 +4171,15 @@
       <c r="E54" s="109" t="s">
         <v>46</v>
       </c>
-      <c r="F54" s="126"/>
-      <c r="G54" s="156"/>
-      <c r="H54" s="145"/>
-      <c r="J54" s="179"/>
-      <c r="K54" s="200"/>
-      <c r="L54" s="180"/>
+      <c r="F54" s="131"/>
+      <c r="G54" s="133"/>
+      <c r="H54" s="136"/>
+      <c r="J54" s="125"/>
+      <c r="K54" s="126"/>
+      <c r="L54" s="127"/>
     </row>
     <row r="55" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="154"/>
+      <c r="B55" s="197"/>
       <c r="C55" s="37" t="s">
         <v>143</v>
       </c>
@@ -4189,36 +4189,36 @@
       <c r="E55" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="F55" s="127"/>
-      <c r="G55" s="157"/>
-      <c r="H55" s="146"/>
-      <c r="J55" s="179"/>
-      <c r="K55" s="200"/>
-      <c r="L55" s="180"/>
+      <c r="F55" s="132"/>
+      <c r="G55" s="129"/>
+      <c r="H55" s="137"/>
+      <c r="J55" s="125"/>
+      <c r="K55" s="126"/>
+      <c r="L55" s="127"/>
     </row>
     <row r="56" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="123">
+      <c r="B56" s="172">
         <v>9</v>
       </c>
-      <c r="C56" s="124"/>
+      <c r="C56" s="173"/>
       <c r="D56" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="E56" s="141" t="s">
+      <c r="E56" s="198" t="s">
         <v>122</v>
       </c>
-      <c r="F56" s="125">
+      <c r="F56" s="130">
         <v>44438</v>
       </c>
-      <c r="G56" s="155">
+      <c r="G56" s="128">
         <v>44438</v>
       </c>
-      <c r="H56" s="144">
+      <c r="H56" s="134">
         <v>1</v>
       </c>
-      <c r="J56" s="179"/>
-      <c r="K56" s="200"/>
-      <c r="L56" s="180"/>
+      <c r="J56" s="125"/>
+      <c r="K56" s="126"/>
+      <c r="L56" s="127"/>
     </row>
     <row r="57" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="35"/>
@@ -4228,40 +4228,40 @@
       <c r="D57" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="E57" s="142"/>
-      <c r="F57" s="127"/>
-      <c r="G57" s="157"/>
-      <c r="H57" s="146"/>
-      <c r="J57" s="179"/>
-      <c r="K57" s="200"/>
-      <c r="L57" s="180"/>
+      <c r="E57" s="199"/>
+      <c r="F57" s="132"/>
+      <c r="G57" s="129"/>
+      <c r="H57" s="137"/>
+      <c r="J57" s="125"/>
+      <c r="K57" s="126"/>
+      <c r="L57" s="127"/>
     </row>
     <row r="58" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="123">
+      <c r="B58" s="172">
         <v>10</v>
       </c>
-      <c r="C58" s="124"/>
+      <c r="C58" s="173"/>
       <c r="D58" s="35" t="s">
         <v>80</v>
       </c>
       <c r="E58" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="F58" s="125">
+      <c r="F58" s="130">
         <v>44439</v>
       </c>
-      <c r="G58" s="155">
+      <c r="G58" s="128">
         <v>44449</v>
       </c>
-      <c r="H58" s="144">
+      <c r="H58" s="134">
         <v>1</v>
       </c>
-      <c r="J58" s="179"/>
-      <c r="K58" s="200"/>
-      <c r="L58" s="180"/>
+      <c r="J58" s="125"/>
+      <c r="K58" s="126"/>
+      <c r="L58" s="127"/>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B59" s="152"/>
+      <c r="B59" s="195"/>
       <c r="C59" s="106" t="s">
         <v>103</v>
       </c>
@@ -4271,15 +4271,15 @@
       <c r="E59" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="F59" s="126"/>
-      <c r="G59" s="156"/>
-      <c r="H59" s="145"/>
-      <c r="J59" s="179"/>
-      <c r="K59" s="200"/>
-      <c r="L59" s="180"/>
+      <c r="F59" s="131"/>
+      <c r="G59" s="133"/>
+      <c r="H59" s="136"/>
+      <c r="J59" s="125"/>
+      <c r="K59" s="126"/>
+      <c r="L59" s="127"/>
     </row>
     <row r="60" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="154"/>
+      <c r="B60" s="197"/>
       <c r="C60" s="38" t="s">
         <v>145</v>
       </c>
@@ -4289,38 +4289,38 @@
       <c r="E60" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="F60" s="127"/>
-      <c r="G60" s="157"/>
-      <c r="H60" s="146"/>
-      <c r="J60" s="181" t="s">
+      <c r="F60" s="132"/>
+      <c r="G60" s="129"/>
+      <c r="H60" s="137"/>
+      <c r="J60" s="138" t="s">
         <v>77</v>
       </c>
-      <c r="K60" s="201"/>
-      <c r="L60" s="182"/>
+      <c r="K60" s="139"/>
+      <c r="L60" s="140"/>
     </row>
     <row r="61" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="123">
+      <c r="B61" s="172">
         <v>11</v>
       </c>
-      <c r="C61" s="124"/>
+      <c r="C61" s="173"/>
       <c r="D61" s="104" t="s">
         <v>199</v>
       </c>
       <c r="E61" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="F61" s="125">
+      <c r="F61" s="130">
         <v>44452</v>
       </c>
-      <c r="G61" s="155">
+      <c r="G61" s="128">
         <v>44453</v>
       </c>
-      <c r="H61" s="144">
+      <c r="H61" s="134">
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B62" s="152"/>
+      <c r="B62" s="195"/>
       <c r="C62" s="106" t="s">
         <v>104</v>
       </c>
@@ -4330,12 +4330,12 @@
       <c r="E62" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="F62" s="126"/>
-      <c r="G62" s="156"/>
-      <c r="H62" s="145"/>
+      <c r="F62" s="131"/>
+      <c r="G62" s="133"/>
+      <c r="H62" s="136"/>
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B63" s="153"/>
+      <c r="B63" s="196"/>
       <c r="C63" s="107" t="s">
         <v>105</v>
       </c>
@@ -4345,12 +4345,12 @@
       <c r="E63" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="F63" s="126"/>
-      <c r="G63" s="156"/>
-      <c r="H63" s="145"/>
+      <c r="F63" s="131"/>
+      <c r="G63" s="133"/>
+      <c r="H63" s="136"/>
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B64" s="153"/>
+      <c r="B64" s="196"/>
       <c r="C64" s="108" t="s">
         <v>106</v>
       </c>
@@ -4360,12 +4360,12 @@
       <c r="E64" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="F64" s="126"/>
-      <c r="G64" s="156"/>
-      <c r="H64" s="145"/>
+      <c r="F64" s="131"/>
+      <c r="G64" s="133"/>
+      <c r="H64" s="136"/>
     </row>
     <row r="65" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="154"/>
+      <c r="B65" s="197"/>
       <c r="C65" s="38" t="s">
         <v>147</v>
       </c>
@@ -4375,33 +4375,33 @@
       <c r="E65" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="F65" s="127"/>
-      <c r="G65" s="157"/>
-      <c r="H65" s="146"/>
+      <c r="F65" s="132"/>
+      <c r="G65" s="129"/>
+      <c r="H65" s="137"/>
     </row>
     <row r="66" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="123">
+      <c r="B66" s="172">
         <v>12</v>
       </c>
-      <c r="C66" s="124"/>
+      <c r="C66" s="173"/>
       <c r="D66" s="104" t="s">
         <v>200</v>
       </c>
       <c r="E66" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="F66" s="125">
+      <c r="F66" s="130">
         <v>44454</v>
       </c>
-      <c r="G66" s="155">
+      <c r="G66" s="128">
         <v>44454</v>
       </c>
-      <c r="H66" s="144">
+      <c r="H66" s="134">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="152"/>
+      <c r="B67" s="195"/>
       <c r="C67" s="115" t="s">
         <v>107</v>
       </c>
@@ -4411,12 +4411,12 @@
       <c r="E67" s="112" t="s">
         <v>129</v>
       </c>
-      <c r="F67" s="126"/>
-      <c r="G67" s="156"/>
-      <c r="H67" s="145"/>
+      <c r="F67" s="131"/>
+      <c r="G67" s="133"/>
+      <c r="H67" s="136"/>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="153"/>
+      <c r="B68" s="196"/>
       <c r="C68" s="116" t="s">
         <v>108</v>
       </c>
@@ -4426,12 +4426,12 @@
       <c r="E68" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="F68" s="126"/>
-      <c r="G68" s="156"/>
-      <c r="H68" s="145"/>
+      <c r="F68" s="131"/>
+      <c r="G68" s="133"/>
+      <c r="H68" s="136"/>
     </row>
     <row r="69" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="154"/>
+      <c r="B69" s="197"/>
       <c r="C69" s="39" t="s">
         <v>109</v>
       </c>
@@ -4441,33 +4441,33 @@
       <c r="E69" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="F69" s="127"/>
-      <c r="G69" s="157"/>
-      <c r="H69" s="146"/>
+      <c r="F69" s="132"/>
+      <c r="G69" s="129"/>
+      <c r="H69" s="137"/>
     </row>
     <row r="70" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="123">
+      <c r="B70" s="172">
         <v>13</v>
       </c>
-      <c r="C70" s="124"/>
+      <c r="C70" s="173"/>
       <c r="D70" s="104" t="s">
         <v>201</v>
       </c>
       <c r="E70" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="F70" s="125">
+      <c r="F70" s="130">
         <v>44455</v>
       </c>
-      <c r="G70" s="155">
+      <c r="G70" s="128">
         <v>44456</v>
       </c>
-      <c r="H70" s="144">
+      <c r="H70" s="134">
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B71" s="152"/>
+      <c r="B71" s="195"/>
       <c r="C71" s="115" t="s">
         <v>110</v>
       </c>
@@ -4477,12 +4477,12 @@
       <c r="E71" s="112" t="s">
         <v>126</v>
       </c>
-      <c r="F71" s="126"/>
-      <c r="G71" s="156"/>
-      <c r="H71" s="145"/>
+      <c r="F71" s="131"/>
+      <c r="G71" s="133"/>
+      <c r="H71" s="136"/>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B72" s="153"/>
+      <c r="B72" s="196"/>
       <c r="C72" s="117" t="s">
         <v>111</v>
       </c>
@@ -4492,12 +4492,12 @@
       <c r="E72" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="F72" s="126"/>
-      <c r="G72" s="156"/>
-      <c r="H72" s="145"/>
+      <c r="F72" s="131"/>
+      <c r="G72" s="133"/>
+      <c r="H72" s="136"/>
     </row>
     <row r="73" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="154"/>
+      <c r="B73" s="197"/>
       <c r="C73" s="39" t="s">
         <v>112</v>
       </c>
@@ -4507,33 +4507,33 @@
       <c r="E73" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="F73" s="127"/>
-      <c r="G73" s="157"/>
-      <c r="H73" s="146"/>
+      <c r="F73" s="132"/>
+      <c r="G73" s="129"/>
+      <c r="H73" s="137"/>
     </row>
     <row r="74" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="123">
+      <c r="B74" s="172">
         <v>14</v>
       </c>
-      <c r="C74" s="124"/>
+      <c r="C74" s="173"/>
       <c r="D74" s="104" t="s">
         <v>202</v>
       </c>
       <c r="E74" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="F74" s="125">
+      <c r="F74" s="130">
         <v>44459</v>
       </c>
-      <c r="G74" s="155">
+      <c r="G74" s="128">
         <v>44470</v>
       </c>
-      <c r="H74" s="144">
-        <v>0.35</v>
+      <c r="H74" s="134">
+        <v>0.5</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="139"/>
+      <c r="B75" s="183"/>
       <c r="C75" s="106" t="s">
         <v>115</v>
       </c>
@@ -4543,12 +4543,12 @@
       <c r="E75" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="F75" s="126"/>
-      <c r="G75" s="156"/>
-      <c r="H75" s="208"/>
+      <c r="F75" s="131"/>
+      <c r="G75" s="133"/>
+      <c r="H75" s="135"/>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="139"/>
+      <c r="B76" s="183"/>
       <c r="C76" s="107" t="s">
         <v>113</v>
       </c>
@@ -4558,12 +4558,12 @@
       <c r="E76" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="F76" s="126"/>
-      <c r="G76" s="156"/>
-      <c r="H76" s="208"/>
+      <c r="F76" s="131"/>
+      <c r="G76" s="133"/>
+      <c r="H76" s="135"/>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B77" s="139"/>
+      <c r="B77" s="183"/>
       <c r="C77" s="108" t="s">
         <v>114</v>
       </c>
@@ -4573,12 +4573,12 @@
       <c r="E77" s="62" t="s">
         <v>155</v>
       </c>
-      <c r="F77" s="126"/>
-      <c r="G77" s="156"/>
-      <c r="H77" s="145"/>
+      <c r="F77" s="131"/>
+      <c r="G77" s="133"/>
+      <c r="H77" s="136"/>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="139"/>
+      <c r="B78" s="183"/>
       <c r="C78" s="107" t="s">
         <v>150</v>
       </c>
@@ -4588,12 +4588,12 @@
       <c r="E78" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="F78" s="126"/>
-      <c r="G78" s="156"/>
-      <c r="H78" s="145"/>
+      <c r="F78" s="131"/>
+      <c r="G78" s="133"/>
+      <c r="H78" s="136"/>
     </row>
     <row r="79" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="140"/>
+      <c r="B79" s="200"/>
       <c r="C79" s="37" t="s">
         <v>154</v>
       </c>
@@ -4603,33 +4603,33 @@
       <c r="E79" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="F79" s="127"/>
-      <c r="G79" s="157"/>
-      <c r="H79" s="146"/>
+      <c r="F79" s="132"/>
+      <c r="G79" s="129"/>
+      <c r="H79" s="137"/>
     </row>
     <row r="80" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="123">
+      <c r="B80" s="172">
         <v>15</v>
       </c>
-      <c r="C80" s="124"/>
+      <c r="C80" s="173"/>
       <c r="D80" s="104" t="s">
         <v>203</v>
       </c>
       <c r="E80" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="F80" s="125">
+      <c r="F80" s="130">
         <v>44473</v>
       </c>
-      <c r="G80" s="155">
+      <c r="G80" s="128">
         <v>44473</v>
       </c>
-      <c r="H80" s="144">
+      <c r="H80" s="134">
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B81" s="139"/>
+      <c r="B81" s="183"/>
       <c r="C81" s="120" t="s">
         <v>175</v>
       </c>
@@ -4639,12 +4639,12 @@
       <c r="E81" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="F81" s="126"/>
-      <c r="G81" s="156"/>
-      <c r="H81" s="208"/>
+      <c r="F81" s="131"/>
+      <c r="G81" s="133"/>
+      <c r="H81" s="135"/>
     </row>
     <row r="82" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="140"/>
+      <c r="B82" s="200"/>
       <c r="C82" s="41" t="s">
         <v>176</v>
       </c>
@@ -4654,28 +4654,28 @@
       <c r="E82" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="F82" s="127"/>
-      <c r="G82" s="157"/>
-      <c r="H82" s="146"/>
+      <c r="F82" s="132"/>
+      <c r="G82" s="129"/>
+      <c r="H82" s="137"/>
     </row>
     <row r="83" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="123">
+      <c r="B83" s="172">
         <v>16</v>
       </c>
-      <c r="C83" s="124"/>
+      <c r="C83" s="173"/>
       <c r="D83" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="E83" s="141" t="s">
+      <c r="E83" s="198" t="s">
         <v>45</v>
       </c>
-      <c r="F83" s="125">
+      <c r="F83" s="130">
         <v>44473</v>
       </c>
-      <c r="G83" s="155">
+      <c r="G83" s="128">
         <v>44473</v>
       </c>
-      <c r="H83" s="144">
+      <c r="H83" s="134">
         <v>0</v>
       </c>
     </row>
@@ -4687,63 +4687,63 @@
       <c r="D84" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="E84" s="142"/>
-      <c r="F84" s="127"/>
-      <c r="G84" s="157"/>
-      <c r="H84" s="146"/>
+      <c r="E84" s="199"/>
+      <c r="F84" s="132"/>
+      <c r="G84" s="129"/>
+      <c r="H84" s="137"/>
     </row>
     <row r="85" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="123">
+      <c r="B85" s="172">
         <v>17</v>
       </c>
-      <c r="C85" s="124"/>
+      <c r="C85" s="173"/>
       <c r="D85" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="E85" s="141" t="s">
+      <c r="E85" s="198" t="s">
         <v>128</v>
       </c>
-      <c r="F85" s="125">
+      <c r="F85" s="130">
         <v>44474</v>
       </c>
-      <c r="G85" s="155">
+      <c r="G85" s="128">
         <v>44474</v>
       </c>
-      <c r="H85" s="144">
+      <c r="H85" s="134">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="139"/>
+      <c r="B86" s="183"/>
       <c r="C86" s="115" t="s">
         <v>117</v>
       </c>
       <c r="D86" s="110" t="s">
         <v>196</v>
       </c>
-      <c r="E86" s="143"/>
-      <c r="F86" s="126"/>
-      <c r="G86" s="156"/>
-      <c r="H86" s="145"/>
+      <c r="E86" s="205"/>
+      <c r="F86" s="131"/>
+      <c r="G86" s="133"/>
+      <c r="H86" s="136"/>
     </row>
     <row r="87" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="140"/>
+      <c r="B87" s="200"/>
       <c r="C87" s="40" t="s">
         <v>118</v>
       </c>
       <c r="D87" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="E87" s="142"/>
-      <c r="F87" s="127"/>
-      <c r="G87" s="157"/>
-      <c r="H87" s="146"/>
+      <c r="E87" s="199"/>
+      <c r="F87" s="132"/>
+      <c r="G87" s="129"/>
+      <c r="H87" s="137"/>
     </row>
     <row r="88" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="123">
+      <c r="B88" s="172">
         <v>18</v>
       </c>
-      <c r="C88" s="124"/>
+      <c r="C88" s="173"/>
       <c r="D88" s="16" t="s">
         <v>96</v>
       </c>
@@ -4761,10 +4761,10 @@
       </c>
     </row>
     <row r="89" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="123">
+      <c r="B89" s="172">
         <v>19</v>
       </c>
-      <c r="C89" s="124"/>
+      <c r="C89" s="173"/>
       <c r="D89" s="17" t="s">
         <v>120</v>
       </c>
@@ -4782,10 +4782,10 @@
       </c>
     </row>
     <row r="90" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="128">
+      <c r="B90" s="206">
         <v>20</v>
       </c>
-      <c r="C90" s="129"/>
+      <c r="C90" s="207"/>
       <c r="D90" s="17" t="s">
         <v>177</v>
       </c>
@@ -4803,113 +4803,163 @@
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B91" s="122"/>
-      <c r="C91" s="122"/>
+      <c r="B91" s="204"/>
+      <c r="C91" s="204"/>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B92" s="122"/>
-      <c r="C92" s="122"/>
+      <c r="B92" s="204"/>
+      <c r="C92" s="204"/>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B93" s="122"/>
-      <c r="C93" s="122"/>
+      <c r="B93" s="204"/>
+      <c r="C93" s="204"/>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B94" s="122"/>
-      <c r="C94" s="122"/>
+      <c r="B94" s="204"/>
+      <c r="C94" s="204"/>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="122"/>
-      <c r="C95" s="122"/>
+      <c r="B95" s="204"/>
+      <c r="C95" s="204"/>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B96" s="122"/>
-      <c r="C96" s="122"/>
+      <c r="B96" s="204"/>
+      <c r="C96" s="204"/>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B97" s="122"/>
-      <c r="C97" s="122"/>
+      <c r="B97" s="204"/>
+      <c r="C97" s="204"/>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="122"/>
-      <c r="C98" s="122"/>
+      <c r="B98" s="204"/>
+      <c r="C98" s="204"/>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B99" s="122"/>
-      <c r="C99" s="122"/>
+      <c r="B99" s="204"/>
+      <c r="C99" s="204"/>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="122"/>
-      <c r="C100" s="122"/>
+      <c r="B100" s="204"/>
+      <c r="C100" s="204"/>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B101" s="122"/>
-      <c r="C101" s="122"/>
+      <c r="B101" s="204"/>
+      <c r="C101" s="204"/>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B102" s="122"/>
-      <c r="C102" s="122"/>
+      <c r="B102" s="204"/>
+      <c r="C102" s="204"/>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B103" s="122"/>
-      <c r="C103" s="122"/>
+      <c r="B103" s="204"/>
+      <c r="C103" s="204"/>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B104" s="122"/>
-      <c r="C104" s="122"/>
+      <c r="B104" s="204"/>
+      <c r="C104" s="204"/>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B105" s="122"/>
-      <c r="C105" s="122"/>
+      <c r="B105" s="204"/>
+      <c r="C105" s="204"/>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B106" s="122"/>
-      <c r="C106" s="122"/>
+      <c r="B106" s="204"/>
+      <c r="C106" s="204"/>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B107" s="122"/>
-      <c r="C107" s="122"/>
+      <c r="B107" s="204"/>
+      <c r="C107" s="204"/>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B108" s="122"/>
-      <c r="C108" s="122"/>
+      <c r="B108" s="204"/>
+      <c r="C108" s="204"/>
     </row>
   </sheetData>
   <mergeCells count="142">
-    <mergeCell ref="J48:L51"/>
-    <mergeCell ref="J53:L59"/>
-    <mergeCell ref="G83:G84"/>
-    <mergeCell ref="F85:F87"/>
-    <mergeCell ref="G85:G87"/>
-    <mergeCell ref="F66:F69"/>
-    <mergeCell ref="G66:G69"/>
-    <mergeCell ref="F70:F73"/>
-    <mergeCell ref="G70:G73"/>
-    <mergeCell ref="F74:F79"/>
-    <mergeCell ref="G74:G79"/>
-    <mergeCell ref="H74:H79"/>
-    <mergeCell ref="H80:H82"/>
-    <mergeCell ref="H83:H84"/>
-    <mergeCell ref="H85:H87"/>
-    <mergeCell ref="H56:H57"/>
-    <mergeCell ref="H58:H60"/>
-    <mergeCell ref="H61:H65"/>
-    <mergeCell ref="H66:H69"/>
-    <mergeCell ref="H70:H73"/>
-    <mergeCell ref="F80:F82"/>
-    <mergeCell ref="G80:G82"/>
-    <mergeCell ref="F83:F84"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J9:L16"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="J18:L22"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="J24:L28"/>
-    <mergeCell ref="J7:L8"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="F9:F15"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="E23:E29"/>
+    <mergeCell ref="F16:F29"/>
+    <mergeCell ref="G16:G29"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="B75:B79"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="E85:E87"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="H9:H15"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="F61:F65"/>
+    <mergeCell ref="G61:G65"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="H16:H29"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="H2:H7"/>
+    <mergeCell ref="F35:F39"/>
+    <mergeCell ref="G35:G39"/>
+    <mergeCell ref="H35:H39"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B2:C7"/>
+    <mergeCell ref="H30:H34"/>
+    <mergeCell ref="G30:G34"/>
+    <mergeCell ref="F30:F34"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="B17:B23"/>
+    <mergeCell ref="B24:C29"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="G9:G15"/>
     <mergeCell ref="J30:L34"/>
     <mergeCell ref="F40:F44"/>
     <mergeCell ref="G40:G44"/>
@@ -4934,90 +4984,40 @@
     <mergeCell ref="H48:H49"/>
     <mergeCell ref="J43:L46"/>
     <mergeCell ref="J52:L52"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="H2:H7"/>
-    <mergeCell ref="F35:F39"/>
-    <mergeCell ref="G35:G39"/>
-    <mergeCell ref="H35:H39"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B2:C7"/>
-    <mergeCell ref="H30:H34"/>
-    <mergeCell ref="G30:G34"/>
-    <mergeCell ref="F30:F34"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="B17:B23"/>
-    <mergeCell ref="B24:C29"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="G9:G15"/>
-    <mergeCell ref="H9:H15"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="B51:B55"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="F61:F65"/>
-    <mergeCell ref="G61:G65"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="H16:H29"/>
-    <mergeCell ref="F16:F29"/>
-    <mergeCell ref="G16:G29"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="B75:B79"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="E85:E87"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="F9:F15"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="E23:E29"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J9:L16"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="J18:L22"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="J24:L28"/>
+    <mergeCell ref="J7:L8"/>
+    <mergeCell ref="J48:L51"/>
+    <mergeCell ref="J53:L59"/>
+    <mergeCell ref="G83:G84"/>
+    <mergeCell ref="F85:F87"/>
+    <mergeCell ref="G85:G87"/>
+    <mergeCell ref="F66:F69"/>
+    <mergeCell ref="G66:G69"/>
+    <mergeCell ref="F70:F73"/>
+    <mergeCell ref="G70:G73"/>
+    <mergeCell ref="F74:F79"/>
+    <mergeCell ref="G74:G79"/>
+    <mergeCell ref="H74:H79"/>
+    <mergeCell ref="H80:H82"/>
+    <mergeCell ref="H83:H84"/>
+    <mergeCell ref="H85:H87"/>
+    <mergeCell ref="H56:H57"/>
+    <mergeCell ref="H58:H60"/>
+    <mergeCell ref="H61:H65"/>
+    <mergeCell ref="H66:H69"/>
+    <mergeCell ref="H70:H73"/>
+    <mergeCell ref="F80:F82"/>
+    <mergeCell ref="G80:G82"/>
+    <mergeCell ref="F83:F84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -5040,263 +5040,263 @@
   <sheetData>
     <row r="1" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B2" s="177"/>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="183" t="s">
+      <c r="B2" s="122"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="184"/>
-      <c r="H2" s="184"/>
-      <c r="I2" s="184"/>
-      <c r="J2" s="184"/>
-      <c r="K2" s="184"/>
-      <c r="L2" s="184"/>
-      <c r="M2" s="184"/>
-      <c r="N2" s="184"/>
-      <c r="O2" s="184"/>
-      <c r="P2" s="184"/>
-      <c r="Q2" s="184"/>
-      <c r="R2" s="184"/>
-      <c r="S2" s="184"/>
-      <c r="T2" s="184"/>
-      <c r="U2" s="184"/>
-      <c r="V2" s="184"/>
-      <c r="W2" s="184"/>
-      <c r="X2" s="184"/>
-      <c r="Y2" s="184"/>
-      <c r="Z2" s="184"/>
-      <c r="AA2" s="184"/>
-      <c r="AB2" s="184"/>
-      <c r="AC2" s="184"/>
-      <c r="AD2" s="184"/>
-      <c r="AE2" s="210"/>
-      <c r="AF2" s="199"/>
-      <c r="AG2" s="199"/>
-      <c r="AH2" s="178"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
+      <c r="P2" s="177"/>
+      <c r="Q2" s="177"/>
+      <c r="R2" s="177"/>
+      <c r="S2" s="177"/>
+      <c r="T2" s="177"/>
+      <c r="U2" s="177"/>
+      <c r="V2" s="177"/>
+      <c r="W2" s="177"/>
+      <c r="X2" s="177"/>
+      <c r="Y2" s="177"/>
+      <c r="Z2" s="177"/>
+      <c r="AA2" s="177"/>
+      <c r="AB2" s="177"/>
+      <c r="AC2" s="177"/>
+      <c r="AD2" s="177"/>
+      <c r="AE2" s="230"/>
+      <c r="AF2" s="123"/>
+      <c r="AG2" s="123"/>
+      <c r="AH2" s="124"/>
     </row>
     <row r="3" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B3" s="179"/>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="180"/>
-      <c r="F3" s="187" t="s">
+      <c r="B3" s="125"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="180" t="s">
         <v>205</v>
       </c>
-      <c r="G3" s="211"/>
-      <c r="H3" s="211"/>
-      <c r="I3" s="211"/>
-      <c r="J3" s="211"/>
-      <c r="K3" s="211"/>
-      <c r="L3" s="211"/>
-      <c r="M3" s="211"/>
-      <c r="N3" s="211"/>
-      <c r="O3" s="211"/>
-      <c r="P3" s="211"/>
-      <c r="Q3" s="211"/>
-      <c r="R3" s="211"/>
-      <c r="S3" s="211"/>
-      <c r="T3" s="211"/>
-      <c r="U3" s="211"/>
-      <c r="V3" s="211"/>
-      <c r="W3" s="211"/>
-      <c r="X3" s="211"/>
-      <c r="Y3" s="211"/>
-      <c r="Z3" s="211"/>
-      <c r="AA3" s="211"/>
-      <c r="AB3" s="211"/>
-      <c r="AC3" s="211"/>
-      <c r="AD3" s="211"/>
-      <c r="AE3" s="189"/>
-      <c r="AF3" s="200"/>
-      <c r="AG3" s="200"/>
-      <c r="AH3" s="180"/>
+      <c r="G3" s="231"/>
+      <c r="H3" s="231"/>
+      <c r="I3" s="231"/>
+      <c r="J3" s="231"/>
+      <c r="K3" s="231"/>
+      <c r="L3" s="231"/>
+      <c r="M3" s="231"/>
+      <c r="N3" s="231"/>
+      <c r="O3" s="231"/>
+      <c r="P3" s="231"/>
+      <c r="Q3" s="231"/>
+      <c r="R3" s="231"/>
+      <c r="S3" s="231"/>
+      <c r="T3" s="231"/>
+      <c r="U3" s="231"/>
+      <c r="V3" s="231"/>
+      <c r="W3" s="231"/>
+      <c r="X3" s="231"/>
+      <c r="Y3" s="231"/>
+      <c r="Z3" s="231"/>
+      <c r="AA3" s="231"/>
+      <c r="AB3" s="231"/>
+      <c r="AC3" s="231"/>
+      <c r="AD3" s="231"/>
+      <c r="AE3" s="182"/>
+      <c r="AF3" s="126"/>
+      <c r="AG3" s="126"/>
+      <c r="AH3" s="127"/>
     </row>
     <row r="4" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B4" s="179"/>
-      <c r="C4" s="200"/>
-      <c r="D4" s="200"/>
-      <c r="E4" s="180"/>
-      <c r="F4" s="187" t="s">
+      <c r="B4" s="125"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="127"/>
+      <c r="F4" s="180" t="s">
         <v>206</v>
       </c>
-      <c r="G4" s="211"/>
-      <c r="H4" s="211"/>
-      <c r="I4" s="211"/>
-      <c r="J4" s="211"/>
-      <c r="K4" s="211"/>
-      <c r="L4" s="211"/>
-      <c r="M4" s="211"/>
-      <c r="N4" s="211"/>
-      <c r="O4" s="211"/>
-      <c r="P4" s="211"/>
-      <c r="Q4" s="211"/>
-      <c r="R4" s="211"/>
-      <c r="S4" s="211"/>
-      <c r="T4" s="211"/>
-      <c r="U4" s="211"/>
-      <c r="V4" s="211"/>
-      <c r="W4" s="211"/>
-      <c r="X4" s="211"/>
-      <c r="Y4" s="211"/>
-      <c r="Z4" s="211"/>
-      <c r="AA4" s="211"/>
-      <c r="AB4" s="211"/>
-      <c r="AC4" s="211"/>
-      <c r="AD4" s="211"/>
-      <c r="AE4" s="189"/>
-      <c r="AF4" s="200"/>
-      <c r="AG4" s="200"/>
-      <c r="AH4" s="180"/>
+      <c r="G4" s="231"/>
+      <c r="H4" s="231"/>
+      <c r="I4" s="231"/>
+      <c r="J4" s="231"/>
+      <c r="K4" s="231"/>
+      <c r="L4" s="231"/>
+      <c r="M4" s="231"/>
+      <c r="N4" s="231"/>
+      <c r="O4" s="231"/>
+      <c r="P4" s="231"/>
+      <c r="Q4" s="231"/>
+      <c r="R4" s="231"/>
+      <c r="S4" s="231"/>
+      <c r="T4" s="231"/>
+      <c r="U4" s="231"/>
+      <c r="V4" s="231"/>
+      <c r="W4" s="231"/>
+      <c r="X4" s="231"/>
+      <c r="Y4" s="231"/>
+      <c r="Z4" s="231"/>
+      <c r="AA4" s="231"/>
+      <c r="AB4" s="231"/>
+      <c r="AC4" s="231"/>
+      <c r="AD4" s="231"/>
+      <c r="AE4" s="182"/>
+      <c r="AF4" s="126"/>
+      <c r="AG4" s="126"/>
+      <c r="AH4" s="127"/>
     </row>
     <row r="5" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B5" s="179"/>
-      <c r="C5" s="200"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="180"/>
-      <c r="F5" s="187" t="s">
+      <c r="B5" s="125"/>
+      <c r="C5" s="126"/>
+      <c r="D5" s="126"/>
+      <c r="E5" s="127"/>
+      <c r="F5" s="180" t="s">
         <v>179</v>
       </c>
-      <c r="G5" s="211"/>
-      <c r="H5" s="211"/>
-      <c r="I5" s="211"/>
-      <c r="J5" s="211"/>
-      <c r="K5" s="211"/>
-      <c r="L5" s="211"/>
-      <c r="M5" s="211"/>
-      <c r="N5" s="211"/>
-      <c r="O5" s="211"/>
-      <c r="P5" s="211"/>
-      <c r="Q5" s="211"/>
-      <c r="R5" s="211"/>
-      <c r="S5" s="211"/>
-      <c r="T5" s="211"/>
-      <c r="U5" s="211"/>
-      <c r="V5" s="211"/>
-      <c r="W5" s="211"/>
-      <c r="X5" s="211"/>
-      <c r="Y5" s="211"/>
-      <c r="Z5" s="211"/>
-      <c r="AA5" s="211"/>
-      <c r="AB5" s="211"/>
-      <c r="AC5" s="211"/>
-      <c r="AD5" s="211"/>
-      <c r="AE5" s="189"/>
-      <c r="AF5" s="200"/>
-      <c r="AG5" s="200"/>
-      <c r="AH5" s="180"/>
+      <c r="G5" s="231"/>
+      <c r="H5" s="231"/>
+      <c r="I5" s="231"/>
+      <c r="J5" s="231"/>
+      <c r="K5" s="231"/>
+      <c r="L5" s="231"/>
+      <c r="M5" s="231"/>
+      <c r="N5" s="231"/>
+      <c r="O5" s="231"/>
+      <c r="P5" s="231"/>
+      <c r="Q5" s="231"/>
+      <c r="R5" s="231"/>
+      <c r="S5" s="231"/>
+      <c r="T5" s="231"/>
+      <c r="U5" s="231"/>
+      <c r="V5" s="231"/>
+      <c r="W5" s="231"/>
+      <c r="X5" s="231"/>
+      <c r="Y5" s="231"/>
+      <c r="Z5" s="231"/>
+      <c r="AA5" s="231"/>
+      <c r="AB5" s="231"/>
+      <c r="AC5" s="231"/>
+      <c r="AD5" s="231"/>
+      <c r="AE5" s="182"/>
+      <c r="AF5" s="126"/>
+      <c r="AG5" s="126"/>
+      <c r="AH5" s="127"/>
     </row>
     <row r="6" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B6" s="179"/>
-      <c r="C6" s="200"/>
-      <c r="D6" s="200"/>
-      <c r="E6" s="180"/>
-      <c r="F6" s="187" t="s">
+      <c r="B6" s="125"/>
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="180" t="s">
         <v>207</v>
       </c>
-      <c r="G6" s="211"/>
-      <c r="H6" s="211"/>
-      <c r="I6" s="211"/>
-      <c r="J6" s="211"/>
-      <c r="K6" s="211"/>
-      <c r="L6" s="211"/>
-      <c r="M6" s="211"/>
-      <c r="N6" s="211"/>
-      <c r="O6" s="211"/>
-      <c r="P6" s="211"/>
-      <c r="Q6" s="211"/>
-      <c r="R6" s="211"/>
-      <c r="S6" s="211"/>
-      <c r="T6" s="211"/>
-      <c r="U6" s="211"/>
-      <c r="V6" s="211"/>
-      <c r="W6" s="211"/>
-      <c r="X6" s="211"/>
-      <c r="Y6" s="211"/>
-      <c r="Z6" s="211"/>
-      <c r="AA6" s="211"/>
-      <c r="AB6" s="211"/>
-      <c r="AC6" s="211"/>
-      <c r="AD6" s="211"/>
-      <c r="AE6" s="189"/>
-      <c r="AF6" s="200"/>
-      <c r="AG6" s="200"/>
-      <c r="AH6" s="180"/>
+      <c r="G6" s="231"/>
+      <c r="H6" s="231"/>
+      <c r="I6" s="231"/>
+      <c r="J6" s="231"/>
+      <c r="K6" s="231"/>
+      <c r="L6" s="231"/>
+      <c r="M6" s="231"/>
+      <c r="N6" s="231"/>
+      <c r="O6" s="231"/>
+      <c r="P6" s="231"/>
+      <c r="Q6" s="231"/>
+      <c r="R6" s="231"/>
+      <c r="S6" s="231"/>
+      <c r="T6" s="231"/>
+      <c r="U6" s="231"/>
+      <c r="V6" s="231"/>
+      <c r="W6" s="231"/>
+      <c r="X6" s="231"/>
+      <c r="Y6" s="231"/>
+      <c r="Z6" s="231"/>
+      <c r="AA6" s="231"/>
+      <c r="AB6" s="231"/>
+      <c r="AC6" s="231"/>
+      <c r="AD6" s="231"/>
+      <c r="AE6" s="182"/>
+      <c r="AF6" s="126"/>
+      <c r="AG6" s="126"/>
+      <c r="AH6" s="127"/>
     </row>
     <row r="7" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="181"/>
-      <c r="C7" s="201"/>
-      <c r="D7" s="201"/>
-      <c r="E7" s="182"/>
-      <c r="F7" s="160" t="s">
+      <c r="B7" s="138"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="140"/>
+      <c r="F7" s="161" t="s">
         <v>208</v>
       </c>
-      <c r="G7" s="161"/>
-      <c r="H7" s="161"/>
-      <c r="I7" s="161"/>
-      <c r="J7" s="161"/>
-      <c r="K7" s="161"/>
-      <c r="L7" s="161"/>
-      <c r="M7" s="161"/>
-      <c r="N7" s="161"/>
-      <c r="O7" s="161"/>
-      <c r="P7" s="161"/>
-      <c r="Q7" s="161"/>
-      <c r="R7" s="161"/>
-      <c r="S7" s="161"/>
-      <c r="T7" s="161"/>
-      <c r="U7" s="161"/>
-      <c r="V7" s="161"/>
-      <c r="W7" s="161"/>
-      <c r="X7" s="161"/>
-      <c r="Y7" s="161"/>
-      <c r="Z7" s="161"/>
-      <c r="AA7" s="161"/>
-      <c r="AB7" s="161"/>
-      <c r="AC7" s="161"/>
-      <c r="AD7" s="161"/>
-      <c r="AE7" s="212"/>
-      <c r="AF7" s="201"/>
-      <c r="AG7" s="201"/>
-      <c r="AH7" s="182"/>
+      <c r="G7" s="162"/>
+      <c r="H7" s="162"/>
+      <c r="I7" s="162"/>
+      <c r="J7" s="162"/>
+      <c r="K7" s="162"/>
+      <c r="L7" s="162"/>
+      <c r="M7" s="162"/>
+      <c r="N7" s="162"/>
+      <c r="O7" s="162"/>
+      <c r="P7" s="162"/>
+      <c r="Q7" s="162"/>
+      <c r="R7" s="162"/>
+      <c r="S7" s="162"/>
+      <c r="T7" s="162"/>
+      <c r="U7" s="162"/>
+      <c r="V7" s="162"/>
+      <c r="W7" s="162"/>
+      <c r="X7" s="162"/>
+      <c r="Y7" s="162"/>
+      <c r="Z7" s="162"/>
+      <c r="AA7" s="162"/>
+      <c r="AB7" s="162"/>
+      <c r="AC7" s="162"/>
+      <c r="AD7" s="162"/>
+      <c r="AE7" s="232"/>
+      <c r="AF7" s="139"/>
+      <c r="AG7" s="139"/>
+      <c r="AH7" s="140"/>
     </row>
     <row r="8" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="175" t="s">
+      <c r="B8" s="170" t="s">
         <v>209</v>
       </c>
-      <c r="C8" s="209"/>
-      <c r="D8" s="209"/>
-      <c r="E8" s="209"/>
-      <c r="F8" s="209"/>
-      <c r="G8" s="209"/>
-      <c r="H8" s="209"/>
-      <c r="I8" s="209"/>
-      <c r="J8" s="209"/>
-      <c r="K8" s="209"/>
-      <c r="L8" s="209"/>
-      <c r="M8" s="209"/>
-      <c r="N8" s="209"/>
-      <c r="O8" s="209"/>
-      <c r="P8" s="209"/>
-      <c r="Q8" s="209"/>
-      <c r="R8" s="209"/>
-      <c r="S8" s="209"/>
-      <c r="T8" s="209"/>
-      <c r="U8" s="209"/>
-      <c r="V8" s="209"/>
-      <c r="W8" s="209"/>
-      <c r="X8" s="209"/>
-      <c r="Y8" s="209"/>
-      <c r="Z8" s="209"/>
-      <c r="AA8" s="209"/>
-      <c r="AB8" s="209"/>
-      <c r="AC8" s="209"/>
-      <c r="AD8" s="209"/>
-      <c r="AE8" s="209"/>
-      <c r="AF8" s="209"/>
-      <c r="AG8" s="209"/>
-      <c r="AH8" s="176"/>
+      <c r="C8" s="229"/>
+      <c r="D8" s="229"/>
+      <c r="E8" s="229"/>
+      <c r="F8" s="229"/>
+      <c r="G8" s="229"/>
+      <c r="H8" s="229"/>
+      <c r="I8" s="229"/>
+      <c r="J8" s="229"/>
+      <c r="K8" s="229"/>
+      <c r="L8" s="229"/>
+      <c r="M8" s="229"/>
+      <c r="N8" s="229"/>
+      <c r="O8" s="229"/>
+      <c r="P8" s="229"/>
+      <c r="Q8" s="229"/>
+      <c r="R8" s="229"/>
+      <c r="S8" s="229"/>
+      <c r="T8" s="229"/>
+      <c r="U8" s="229"/>
+      <c r="V8" s="229"/>
+      <c r="W8" s="229"/>
+      <c r="X8" s="229"/>
+      <c r="Y8" s="229"/>
+      <c r="Z8" s="229"/>
+      <c r="AA8" s="229"/>
+      <c r="AB8" s="229"/>
+      <c r="AC8" s="229"/>
+      <c r="AD8" s="229"/>
+      <c r="AE8" s="229"/>
+      <c r="AF8" s="229"/>
+      <c r="AG8" s="229"/>
+      <c r="AH8" s="171"/>
     </row>
     <row r="9" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
@@ -5336,41 +5336,41 @@
     <row r="10" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B10" s="42"/>
       <c r="C10" s="10"/>
-      <c r="D10" s="215" t="s">
+      <c r="D10" s="211" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="216"/>
-      <c r="F10" s="216"/>
-      <c r="G10" s="216"/>
-      <c r="H10" s="216"/>
-      <c r="I10" s="216"/>
-      <c r="J10" s="216"/>
+      <c r="E10" s="212"/>
+      <c r="F10" s="212"/>
+      <c r="G10" s="212"/>
+      <c r="H10" s="212"/>
+      <c r="I10" s="212"/>
+      <c r="J10" s="212"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="42"/>
       <c r="N10" s="10"/>
-      <c r="O10" s="215" t="s">
+      <c r="O10" s="211" t="s">
         <v>15</v>
       </c>
-      <c r="P10" s="216"/>
-      <c r="Q10" s="216"/>
-      <c r="R10" s="216"/>
-      <c r="S10" s="216"/>
-      <c r="T10" s="216"/>
-      <c r="U10" s="216"/>
+      <c r="P10" s="212"/>
+      <c r="Q10" s="212"/>
+      <c r="R10" s="212"/>
+      <c r="S10" s="212"/>
+      <c r="T10" s="212"/>
+      <c r="U10" s="212"/>
       <c r="V10" s="10"/>
       <c r="W10" s="43"/>
       <c r="X10" s="42"/>
       <c r="Y10" s="10"/>
-      <c r="Z10" s="215" t="s">
+      <c r="Z10" s="211" t="s">
         <v>20</v>
       </c>
-      <c r="AA10" s="216"/>
-      <c r="AB10" s="216"/>
-      <c r="AC10" s="216"/>
-      <c r="AD10" s="216"/>
-      <c r="AE10" s="216"/>
-      <c r="AF10" s="216"/>
+      <c r="AA10" s="212"/>
+      <c r="AB10" s="212"/>
+      <c r="AC10" s="212"/>
+      <c r="AD10" s="212"/>
+      <c r="AE10" s="212"/>
+      <c r="AF10" s="212"/>
       <c r="AG10" s="10"/>
       <c r="AH10" s="43"/>
     </row>
@@ -5965,7 +5965,7 @@
     </row>
     <row r="20" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B20" s="42"/>
-      <c r="C20" s="221">
+      <c r="C20" s="217">
         <v>16</v>
       </c>
       <c r="D20" s="6" t="s">
@@ -5980,7 +5980,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="10"/>
       <c r="M20" s="42"/>
-      <c r="N20" s="227">
+      <c r="N20" s="223">
         <v>6</v>
       </c>
       <c r="O20" s="8" t="s">
@@ -5995,7 +5995,7 @@
       <c r="V20" s="3"/>
       <c r="W20" s="43"/>
       <c r="X20" s="42"/>
-      <c r="Y20" s="217">
+      <c r="Y20" s="213">
         <v>4</v>
       </c>
       <c r="Z20" s="8" t="s">
@@ -6012,7 +6012,7 @@
     </row>
     <row r="21" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="42"/>
-      <c r="C21" s="222"/>
+      <c r="C21" s="218"/>
       <c r="D21" s="7" t="s">
         <v>10</v>
       </c>
@@ -6025,7 +6025,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="10"/>
       <c r="M21" s="42"/>
-      <c r="N21" s="228"/>
+      <c r="N21" s="224"/>
       <c r="O21" s="9" t="s">
         <v>12</v>
       </c>
@@ -6038,7 +6038,7 @@
       <c r="V21" s="5"/>
       <c r="W21" s="43"/>
       <c r="X21" s="42"/>
-      <c r="Y21" s="218"/>
+      <c r="Y21" s="214"/>
       <c r="Z21" s="9" t="s">
         <v>12</v>
       </c>
@@ -6053,7 +6053,7 @@
     </row>
     <row r="22" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B22" s="42"/>
-      <c r="C22" s="223">
+      <c r="C22" s="219">
         <v>23</v>
       </c>
       <c r="D22" s="6" t="s">
@@ -6068,7 +6068,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="10"/>
       <c r="M22" s="42"/>
-      <c r="N22" s="229">
+      <c r="N22" s="225">
         <v>13</v>
       </c>
       <c r="O22" s="8" t="s">
@@ -6083,7 +6083,7 @@
       <c r="V22" s="3"/>
       <c r="W22" s="43"/>
       <c r="X22" s="42"/>
-      <c r="Y22" s="219">
+      <c r="Y22" s="215">
         <v>8</v>
       </c>
       <c r="Z22" s="8" t="s">
@@ -6100,7 +6100,7 @@
     </row>
     <row r="23" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="42"/>
-      <c r="C23" s="224"/>
+      <c r="C23" s="220"/>
       <c r="D23" s="7" t="s">
         <v>12</v>
       </c>
@@ -6113,7 +6113,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="10"/>
       <c r="M23" s="42"/>
-      <c r="N23" s="230"/>
+      <c r="N23" s="226"/>
       <c r="O23" s="9" t="s">
         <v>12</v>
       </c>
@@ -6126,7 +6126,7 @@
       <c r="V23" s="5"/>
       <c r="W23" s="43"/>
       <c r="X23" s="42"/>
-      <c r="Y23" s="220"/>
+      <c r="Y23" s="216"/>
       <c r="Z23" s="9" t="s">
         <v>31</v>
       </c>
@@ -6141,7 +6141,7 @@
     </row>
     <row r="24" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B24" s="42"/>
-      <c r="C24" s="225">
+      <c r="C24" s="221">
         <v>30</v>
       </c>
       <c r="D24" s="8" t="s">
@@ -6156,7 +6156,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="10"/>
       <c r="M24" s="42"/>
-      <c r="N24" s="231">
+      <c r="N24" s="227">
         <v>20</v>
       </c>
       <c r="O24" s="8" t="s">
@@ -6184,7 +6184,7 @@
     </row>
     <row r="25" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="42"/>
-      <c r="C25" s="226"/>
+      <c r="C25" s="222"/>
       <c r="D25" s="9" t="s">
         <v>12</v>
       </c>
@@ -6197,7 +6197,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="10"/>
       <c r="M25" s="42"/>
-      <c r="N25" s="232"/>
+      <c r="N25" s="228"/>
       <c r="O25" s="9" t="s">
         <v>12</v>
       </c>
@@ -6234,7 +6234,7 @@
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="M26" s="42"/>
-      <c r="N26" s="213">
+      <c r="N26" s="209">
         <v>27</v>
       </c>
       <c r="O26" s="8" t="s">
@@ -6273,7 +6273,7 @@
       <c r="K27" s="10"/>
       <c r="L27" s="10"/>
       <c r="M27" s="42"/>
-      <c r="N27" s="214"/>
+      <c r="N27" s="210"/>
       <c r="O27" s="9" t="s">
         <v>12</v>
       </c>
@@ -6334,6 +6334,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B2:E7"/>
+    <mergeCell ref="B8:AH8"/>
+    <mergeCell ref="AF2:AH7"/>
+    <mergeCell ref="F2:AE2"/>
+    <mergeCell ref="F3:AE3"/>
+    <mergeCell ref="F4:AE4"/>
+    <mergeCell ref="F5:AE5"/>
+    <mergeCell ref="F6:AE6"/>
+    <mergeCell ref="F7:AE7"/>
     <mergeCell ref="N26:N27"/>
     <mergeCell ref="Z10:AF10"/>
     <mergeCell ref="Y20:Y21"/>
@@ -6346,15 +6355,6 @@
     <mergeCell ref="N20:N21"/>
     <mergeCell ref="N22:N23"/>
     <mergeCell ref="N24:N25"/>
-    <mergeCell ref="B2:E7"/>
-    <mergeCell ref="B8:AH8"/>
-    <mergeCell ref="AF2:AH7"/>
-    <mergeCell ref="F2:AE2"/>
-    <mergeCell ref="F3:AE3"/>
-    <mergeCell ref="F4:AE4"/>
-    <mergeCell ref="F5:AE5"/>
-    <mergeCell ref="F6:AE6"/>
-    <mergeCell ref="F7:AE7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>